<commit_message>
update ICSME and ASE-Demo papers
</commit_message>
<xml_diff>
--- a/src/li-publications.xlsx
+++ b/src/li-publications.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/li.li/git_workspace/lilicoding.github.io/src/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27960" yWindow="460" windowWidth="34540" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="30160" yWindow="6540" windowWidth="34540" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
   <si>
     <t>TITLE</t>
   </si>
@@ -261,6 +256,15 @@
   </si>
   <si>
     <t>acceptance rate: 29% (37/127)</t>
+  </si>
+  <si>
+    <t>li2016reflection</t>
+  </si>
+  <si>
+    <t>Reflection-Aware Static Analysis of Android Apps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 31st IEEE/ACM International Conference on Automated Software Engineering, Demo Track (ASE 2016) </t>
   </si>
 </sst>
 </file>
@@ -302,8 +306,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="203">
+  <cellStyleXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -513,7 +521,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="203">
+  <cellStyles count="207">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -615,6 +623,8 @@
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -716,6 +726,8 @@
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1050,13 +1062,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
@@ -1068,7 +1080,7 @@
     <col min="11" max="11" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1103,7 +1115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1126,7 +1138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1149,7 +1161,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1172,7 +1184,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1195,7 +1207,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1227,7 +1239,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1256,7 +1268,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1279,7 +1291,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1305,7 +1317,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1331,7 +1343,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1354,7 +1366,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1383,7 +1395,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1406,12 +1418,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1420,23 +1429,54 @@
         <v>2016</v>
       </c>
       <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>2016</v>
+      </c>
+      <c r="E15" t="s">
         <v>74</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>75</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>77</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" t="s">
         <v>76</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K15" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update a little bit
</commit_message>
<xml_diff>
--- a/src/li-publications.xlsx
+++ b/src/li-publications.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27809"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/li.li/Project/github/lilicoding.github.io/src/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30160" yWindow="6540" windowWidth="34540" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="30160" yWindow="6540" windowWidth="37040" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
   <si>
     <t>TITLE</t>
   </si>
@@ -265,13 +273,31 @@
   </si>
   <si>
     <t xml:space="preserve">The 31st IEEE/ACM International Conference on Automated Software Engineering, Demo Track (ASE 2016) </t>
+  </si>
+  <si>
+    <t>Li, Li and Li, Daoyuan and Bissyand{\'e}, Tegawend{\'e} F and Klein, Jacques and Le Traon, Yves and Lo, David and Cavallaro, Lorenzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding Android App Piggybacking: A Systematic Study of Malicious Code Grafting </t>
+  </si>
+  <si>
+    <t>IEEE Transactions on Information Forensics &amp; Security (TIFS)</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li Li, Daoyuan Li, Tegawendé F. Bissyandé, Jacques Klein, Yves Le Traon, David Lo and Lorenzo Cavallaro </t>
+  </si>
+  <si>
+    <t>li2017understanding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -287,6 +313,10 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Verdana,Italic"/>
     </font>
   </fonts>
   <fills count="2">
@@ -515,11 +545,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="207">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1062,17 +1093,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="5" max="6" width="94.6640625" customWidth="1"/>
+    <col min="5" max="5" width="94.6640625" customWidth="1"/>
+    <col min="6" max="6" width="105.33203125" customWidth="1"/>
     <col min="7" max="7" width="83.5" customWidth="1"/>
     <col min="8" max="8" width="97.33203125" customWidth="1"/>
     <col min="9" max="9" width="36.1640625" customWidth="1"/>
@@ -1080,7 +1112,7 @@
     <col min="11" max="11" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1115,7 +1147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1138,7 +1170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1161,7 +1193,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1184,7 +1216,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1207,7 +1239,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1239,7 +1271,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1268,7 +1300,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1291,7 +1323,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1317,7 +1349,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1343,7 +1375,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1366,7 +1398,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1395,7 +1427,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1418,7 +1450,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1441,7 +1473,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -1468,15 +1500,36 @@
       </c>
       <c r="K15" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>2017</v>
+      </c>
+      <c r="E16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>